<commit_message>
Fix bug in MonthTemplate
</commit_message>
<xml_diff>
--- a/SolarRiediDataStoring/ReportingWPF/Template/MonthTemplate.xlsx
+++ b/SolarRiediDataStoring/ReportingWPF/Template/MonthTemplate.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Grafica" sheetId="3" r:id="rId1"/>
@@ -5578,7 +5578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R51" sqref="R51"/>
     </sheetView>
   </sheetViews>
@@ -5593,8 +5593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD452"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5661,24 +5661,31 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <f>rawData!C1/1000</f>
         <v>0</v>
       </c>
       <c r="D2">
+        <f>rawData!D1/1000</f>
         <v>0</v>
       </c>
       <c r="E2">
+        <f>rawData!E1/1000</f>
         <v>0</v>
       </c>
       <c r="F2">
+        <f>rawData!F1/1000</f>
         <v>0</v>
       </c>
       <c r="G2">
+        <f>rawData!G1/1000</f>
         <v>0</v>
       </c>
       <c r="H2">
+        <f>rawData!H1/1000</f>
         <v>0</v>
       </c>
       <c r="I2">
+        <f t="shared" ref="I2:I32" si="0">SUM(C2:H2)</f>
         <v>0</v>
       </c>
       <c r="K2">
@@ -5690,19 +5697,19 @@
         <v>#DIV/0!</v>
       </c>
       <c r="M2" t="e">
-        <f t="shared" ref="M2:P2" si="0">D2/$K2</f>
+        <f t="shared" ref="M2:P2" si="1">D2/$K2</f>
         <v>#DIV/0!</v>
       </c>
       <c r="N2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="O2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="P2" t="e">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Q2" t="e">
@@ -5746,7 +5753,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I32" si="1">SUM(C3:H3)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K3">
@@ -5814,7 +5821,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K4">
@@ -5882,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K5">
@@ -5950,7 +5957,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K6">
@@ -6018,7 +6025,7 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K7">
@@ -6086,7 +6093,7 @@
         <v>0</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K8">
@@ -6154,7 +6161,7 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K9">
@@ -6222,7 +6229,7 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K10">
@@ -6290,7 +6297,7 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K11">
@@ -6358,7 +6365,7 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K12">
@@ -6426,7 +6433,7 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K13">
@@ -6494,7 +6501,7 @@
         <v>0</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K14">
@@ -6562,7 +6569,7 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K15">
@@ -6630,7 +6637,7 @@
         <v>0</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K16">
@@ -6698,7 +6705,7 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K17">
@@ -6766,7 +6773,7 @@
         <v>0</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K18">
@@ -6834,7 +6841,7 @@
         <v>0</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K19">
@@ -6902,7 +6909,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K20">
@@ -6970,7 +6977,7 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K21">
@@ -7038,7 +7045,7 @@
         <v>0</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K22">
@@ -7106,7 +7113,7 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K23">
@@ -7174,7 +7181,7 @@
         <v>0</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K24">
@@ -7242,7 +7249,7 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K25">
@@ -7310,7 +7317,7 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K26">
@@ -7378,7 +7385,7 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K27">
@@ -7446,7 +7453,7 @@
         <v>0</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K28">
@@ -7514,7 +7521,7 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K29">
@@ -7582,7 +7589,7 @@
         <v>0</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K30">
@@ -7650,7 +7657,7 @@
         <v>0</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K31">
@@ -7718,7 +7725,7 @@
         <v>0</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="K32">
@@ -7762,8 +7769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>